<commit_message>
rework architettura di comunicazione
</commit_message>
<xml_diff>
--- a/tesi references.xlsx
+++ b/tesi references.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enrim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enrim\Desktop\Tesi-Laurea-Triennale-Informatica-Unimore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC38D991-51A9-421F-840D-2378B07AA5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48841FF3-5C1E-45A7-AD2E-D445161EBEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22860" yWindow="1065" windowWidth="21600" windowHeight="14745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="570" windowWidth="21600" windowHeight="14745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CITAZIONE</t>
   </si>
@@ -40,6 +40,19 @@
   </si>
   <si>
     <t>L'a. i. consiste nell'impiego coordinato di soluzioni tecnologiche allo scopo di sostituire gran parte del lavoro umano con dispositivi diversi</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/an/slla272d/slla272d.pdf?ts=1694247848901</t>
+  </si>
+  <si>
+    <t>The RS-485 standards suggests that its nodes be networked in a daisy-chain, also known as party line or bus topology. In this topology, the participating drivers, receivers, and transceivers connect to a main cable trunk via short network stubs. The interface bus can be designed for full-duplex or half-duplex transmission</t>
+  </si>
+  <si>
+    <t>https://www.overdigit.com/data/Blog/RS485-Modbus/Protocollo%20Modbus%20su%20RS485.pdf</t>
+  </si>
+  <si>
+    <t>Il protocollo Modbus è di tipo Master/Slave e quindi nella rete è presente sempre e solo un dispositivo Master che gestisce la comunicazione nei confronti di uno o più dispositivi Slave.
+Ogni scambio di informazioni è originato dal Master il quale comunica sul bus di campo contente una particolare richiesta, normalmente un comando di lettura o di scrittura delle informazioni contenute in uno degli Slave. Tutti gli Slave sono normalmente in ricezione ed ascoltano le richieste del Master. Solo lo specifico Slave interrogato cattura le informazioni inviate dal Master, provvede all’esecuzione del comando e risponde al Master inviando a sua volta le proprie informazioni sulla rete.</t>
   </si>
 </sst>
 </file>
@@ -97,14 +110,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -389,7 +424,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,89 +445,101 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>45178</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+    <row r="3" spans="1:3" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45178</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
@@ -569,8 +616,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{6A57153D-24D1-4F54-AA93-17E41FB454C5}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{03C82F1C-DEDF-4750-8D8F-40D9C3C2485E}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{C9725B22-827B-4EF4-942C-488FDA306916}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed footnotes for images
</commit_message>
<xml_diff>
--- a/tesi references.xlsx
+++ b/tesi references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enrim\Desktop\Tesi-Laurea-Triennale-Informatica-Unimore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48841FF3-5C1E-45A7-AD2E-D445161EBEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F57CE65-5524-4BD8-A393-C6DEB4550A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="570" windowWidth="21600" windowHeight="14745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27045" yWindow="450" windowWidth="21600" windowHeight="14745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>CITAZIONE</t>
   </si>
@@ -53,6 +53,9 @@
   <si>
     <t>Il protocollo Modbus è di tipo Master/Slave e quindi nella rete è presente sempre e solo un dispositivo Master che gestisce la comunicazione nei confronti di uno o più dispositivi Slave.
 Ogni scambio di informazioni è originato dal Master il quale comunica sul bus di campo contente una particolare richiesta, normalmente un comando di lettura o di scrittura delle informazioni contenute in uno degli Slave. Tutti gli Slave sono normalmente in ricezione ed ascoltano le richieste del Master. Solo lo specifico Slave interrogato cattura le informazioni inviate dal Master, provvede all’esecuzione del comando e risponde al Master inviando a sua volta le proprie informazioni sulla rete.</t>
+  </si>
+  <si>
+    <t>Figura 2: Struttura del frame Modbus in modalità RTU, consultato il 10 settembre 2023,  https://development.libelium.com/modbus_networking_guide/introduction</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +482,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
     </row>

</xml_diff>